<commit_message>
mời sinh viên tham gia lớp học phần và tạo tài khoản khi sinh viên có email và mssv chưa tồn tại trong hệ thống
</commit_message>
<xml_diff>
--- a/HeThongQuanLyBaiGiang/public/LopHocPhan/Template_Import_Student.xlsx
+++ b/HeThongQuanLyBaiGiang/public/LopHocPhan/Template_Import_Student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN\HeThongQuanLyBaiGiang\HeThongQuanLyBaiGiang\public\LopHocPhan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBC3494-4D7C-4745-92F6-B6F879E5FDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7CE495-1CDD-4E0E-AA67-077FB363F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AEA291F1-AB94-4461-8709-9F21CA313E9D}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,32 +84,6 @@
       <b/>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -154,11 +128,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -169,20 +142,13 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85EC221-E38F-4D92-8F87-E25FF61D6258}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,46 +474,28 @@
     <col min="2" max="2" width="20.69921875" style="2" customWidth="1"/>
     <col min="3" max="3" width="35.69921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.69921875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.69921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.69921875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Email không hợp lệ&quot;" error="&quot;Vui lòng nhập đúng định dạng email&quot;" sqref="C2:C1048576" xr:uid="{D55C4C6C-064F-4EA4-AF39-2E89502E9B11}">
-      <formula1>AND(ISNUMBER(FIND("@", C2)), ISNUMBER(FIND(".", C2)), FIND("@", C2) &lt; FIND(".", C2))</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Ngày sinh không hợp lệ&quot;" error="&quot;Vui lòng nhập ngày sinh theo định dạng dd/MM/yyyy và lớn hơn 17 tuổi&quot;" sqref="D2:D1048576" xr:uid="{FF14C7E3-97AD-4825-9F22-8CBDF8A35390}">
-      <formula1>TODAY()-365.25*17</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Giới tính không hợp lệ&quot;" error="&quot;Vui lòng chọn hoặc nhập lại giới tính, chỉ chấp nhận các giá trị Nam, Nữ, Khác&quot;" sqref="E2:E1048576" xr:uid="{8734FDEF-7169-473F-8A69-A3AF1222F9E5}">
-      <formula1>"Nam,Nữ,Khác"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Mã số sinh viên không hợp lệ&quot;" error="&quot;Vui lòng nhập lại MSSV, chỉ chấp nhận giá trị là số và có 10 ký tự&quot;" sqref="B2:B1048576" xr:uid="{B338C1AC-F74F-4C07-BCF3-4DBDD001BFE3}">
-      <formula1>AND(LEN(B2)=10, ISNUMBER(--B2))</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>